<commit_message>
Prenotazione di un volo diagramma delle attività
</commit_message>
<xml_diff>
--- a/BackLog1.xlsx
+++ b/BackLog1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t xml:space="preserve">Task name</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t xml:space="preserve">produzione diagrammi attività specifici </t>
-  </si>
-  <si>
-    <t xml:space="preserve">To do</t>
   </si>
   <si>
     <t xml:space="preserve">Stefani e Zheng</t>
@@ -119,15 +116,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$€-410]\ #,##0.00;[RED]\-[$€-410]\ #,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -145,21 +142,11 @@
       <family val="0"/>
     </font>
     <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <name val="Lucida Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Lucida Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -191,7 +178,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -215,14 +202,6 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -233,7 +212,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -242,17 +221,13 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Risultato" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Risultato2" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Intestazione" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Intestazione1" xfId="23" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -325,7 +300,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -384,7 +359,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>11</v>
@@ -412,7 +387,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>14</v>
@@ -426,7 +401,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -468,7 +443,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
@@ -482,35 +457,35 @@
         <v>25</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>

</xml_diff>